<commit_message>
feat(python): add "pyxlsb" engine support to `read_excel` (for excel binary workbook files) (#11248)
</commit_message>
<xml_diff>
--- a/py-polars/tests/unit/io/files/example.xlsx
+++ b/py-polars/tests/unit/io/files/example.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elvis/GitHub/polars/py-polars/tests/unit/io/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a13107q/PycharmProjects/polars/py-polars/tests/unit/io/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89929A88-0E13-A846-A4D4-2FD349F8179E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{856AF825-6EBE-EF42-AD0D-055AF191BC44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6920" yWindow="9160" windowWidth="22100" windowHeight="14480" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37900" yWindow="20060" windowWidth="22100" windowHeight="14480" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test1" sheetId="1" r:id="rId1"/>
     <sheet name="test2" sheetId="2" r:id="rId2"/>
     <sheet name="test3" sheetId="3" r:id="rId3"/>
     <sheet name="test4" sheetId="4" r:id="rId4"/>
+    <sheet name="test5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>hello</t>
   </si>
@@ -74,20 +75,38 @@
   </si>
   <si>
     <t>:))</t>
+  </si>
+  <si>
+    <t>val</t>
+  </si>
+  <si>
+    <t>dt</t>
+  </si>
+  <si>
+    <t>dtm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -110,13 +129,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -128,22 +173,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{B646C9DC-CF89-1844-B1F6-969631BBBD7F}"/>
+    <cellStyle name="Normal 3" xfId="3" xr:uid="{D65B7284-0216-A64A-AC6B-2B9C645B72D5}"/>
     <cellStyle name="Per cent 2" xfId="2" xr:uid="{2DCABF6C-A3B8-464F-B265-6E3D296E4444}"/>
   </cellStyles>
   <dxfs count="8">
@@ -308,9 +363,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F0FCAA37-C0F1-2E4A-9449-70A700D0CF87}" name="Table1" displayName="Table1" ref="B5:D12" totalsRowCount="1" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="B5:D11" xr:uid="{4B333195-25A9-3A4B-905B-074BF2160312}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{FAEF52EA-738E-B848-9223-816DF50E209A}" name="cardinality" totalsRowLabel="Total" dataDxfId="5" totalsRowDxfId="2" totalsRowCellStyle="Normal 2"/>
-    <tableColumn id="2" xr3:uid="{80EF63AC-AD6E-B049-885B-64EE1A7B65E2}" name="rows_by_key" dataDxfId="4" totalsRowDxfId="1" totalsRowCellStyle="Normal 2"/>
-    <tableColumn id="3" xr3:uid="{24FD4732-0F67-2A4E-BDE8-D215A7302179}" name="iter_groups" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="0" totalsRowCellStyle="Normal 2"/>
+    <tableColumn id="1" xr3:uid="{FAEF52EA-738E-B848-9223-816DF50E209A}" name="cardinality" totalsRowLabel="Total" dataDxfId="5" totalsRowDxfId="4" totalsRowCellStyle="Normal 2"/>
+    <tableColumn id="2" xr3:uid="{80EF63AC-AD6E-B049-885B-64EE1A7B65E2}" name="rows_by_key" dataDxfId="3" totalsRowDxfId="2" totalsRowCellStyle="Normal 2"/>
+    <tableColumn id="3" xr3:uid="{24FD4732-0F67-2A4E-BDE8-D215A7302179}" name="iter_groups" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0" totalsRowCellStyle="Normal 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -615,14 +670,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
     </row>
@@ -650,14 +703,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
+      <c r="A1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
@@ -685,7 +736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE632952-247C-8548-B0FE-C295508C7F03}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -1170,4 +1221,58 @@
     <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;8&amp;K737373 Classification: Public</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96CCBD78-1211-5646-88B1-B0B72F3EDB7B}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="7"/>
+    <col min="3" max="3" width="4.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="9">
+        <v>36525.438020833331</v>
+      </c>
+      <c r="B2" s="11">
+        <v>45292</v>
+      </c>
+      <c r="C2" s="8">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="9">
+        <v>40462.509189814817</v>
+      </c>
+      <c r="B3" s="11">
+        <v>43319</v>
+      </c>
+      <c r="C3" s="8">
+        <v>-0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>